<commit_message>
update job search sheet
</commit_message>
<xml_diff>
--- a/docs/job_search.xlsx
+++ b/docs/job_search.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\portfolio\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705C0D06-BFDD-466A-A571-0EBFA8C10577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0EFD91-A381-4093-920B-5F7416FBB2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Applications" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$K$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Applications!$A$2:$K$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="109">
   <si>
     <t>applied_on</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>workday</t>
+  </si>
+  <si>
+    <t>Nitro</t>
+  </si>
+  <si>
+    <t>networking</t>
   </si>
 </sst>
 </file>
@@ -738,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -845,11 +851,11 @@
       </c>
       <c r="J3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K3" s="6">
         <f ca="1">DATEDIF(A3,J3,"D")</f>
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -990,11 +996,11 @@
       </c>
       <c r="J7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1171,11 +1177,11 @@
       </c>
       <c r="J12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1316,11 +1322,11 @@
       </c>
       <c r="J16" s="4">
         <f ca="1">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K16" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1353,11 +1359,11 @@
       </c>
       <c r="J17" s="4">
         <f ca="1">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K17" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1390,11 +1396,11 @@
       </c>
       <c r="J18" s="4">
         <f ca="1">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K18" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1463,11 +1469,11 @@
       </c>
       <c r="J20" s="4">
         <f ca="1">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K20" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1536,11 +1542,11 @@
       </c>
       <c r="J22" s="4">
         <f ca="1">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K22" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1573,11 +1579,11 @@
       </c>
       <c r="J23" s="4">
         <f ca="1">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K23" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1646,11 +1652,11 @@
       </c>
       <c r="J25" s="4">
         <f t="shared" ref="J25:J34" ca="1" si="1">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K25" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1683,11 +1689,11 @@
       </c>
       <c r="J26" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K26" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1720,11 +1726,11 @@
       </c>
       <c r="J27" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K27" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1757,11 +1763,11 @@
       </c>
       <c r="J28" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K28" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1794,11 +1800,11 @@
       </c>
       <c r="J29" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K29" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1831,11 +1837,11 @@
       </c>
       <c r="J30" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K30" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1868,11 +1874,11 @@
       </c>
       <c r="J31" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K31" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1905,11 +1911,11 @@
       </c>
       <c r="J32" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K32" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1942,11 +1948,11 @@
       </c>
       <c r="J33" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K33" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1979,11 +1985,11 @@
       </c>
       <c r="J34" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K34" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2016,11 +2022,11 @@
       </c>
       <c r="J35" s="4">
         <f t="shared" ref="J35:J41" ca="1" si="2">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K35" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2053,11 +2059,11 @@
       </c>
       <c r="J36" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K36" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2122,15 +2128,14 @@
         <v>70</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J38" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>45049</v>
-      </c>
-      <c r="K38" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>54</v>
+      </c>
+      <c r="J38" s="7">
+        <v>45057</v>
+      </c>
+      <c r="K38" s="8">
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -2163,11 +2168,11 @@
       </c>
       <c r="J39" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K39" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -2200,11 +2205,11 @@
       </c>
       <c r="J40" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K40" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2237,11 +2242,11 @@
       </c>
       <c r="J41" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K41" s="6">
-        <f t="shared" ref="K41:K43" ca="1" si="3">DATEDIF(A41,J41,"d")</f>
-        <v>7</v>
+        <f t="shared" ref="K41:K44" ca="1" si="3">DATEDIF(A41,J41,"d")</f>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -2310,11 +2315,48 @@
       </c>
       <c r="J43" s="4">
         <f ca="1">TODAY()</f>
-        <v>45049</v>
+        <v>45059</v>
       </c>
       <c r="K43" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>45048</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H44" s="1">
+        <v>80</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J44" s="4">
+        <f ca="1">TODAY()</f>
+        <v>45059</v>
+      </c>
+      <c r="K44" s="6">
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update job search
</commit_message>
<xml_diff>
--- a/docs/job_search.xlsx
+++ b/docs/job_search.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\portfolio\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0EFD91-A381-4093-920B-5F7416FBB2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196C619F-2695-4618-BAE7-8B271828516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K32" sqref="J32:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -851,11 +851,11 @@
       </c>
       <c r="J3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K3" s="6">
         <f ca="1">DATEDIF(A3,J3,"D")</f>
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -996,11 +996,11 @@
       </c>
       <c r="J7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1177,11 +1177,11 @@
       </c>
       <c r="J12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1322,11 +1322,11 @@
       </c>
       <c r="J16" s="4">
         <f ca="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K16" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1359,11 +1359,11 @@
       </c>
       <c r="J17" s="4">
         <f ca="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K17" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1396,11 +1396,11 @@
       </c>
       <c r="J18" s="4">
         <f ca="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K18" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1469,11 +1469,11 @@
       </c>
       <c r="J20" s="4">
         <f ca="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K20" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1542,11 +1542,11 @@
       </c>
       <c r="J22" s="4">
         <f ca="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K22" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1579,11 +1579,11 @@
       </c>
       <c r="J23" s="4">
         <f ca="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K23" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1652,11 +1652,11 @@
       </c>
       <c r="J25" s="4">
         <f t="shared" ref="J25:J34" ca="1" si="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K25" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1689,11 +1689,11 @@
       </c>
       <c r="J26" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K26" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1726,11 +1726,11 @@
       </c>
       <c r="J27" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K27" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1763,11 +1763,11 @@
       </c>
       <c r="J28" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K28" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1800,11 +1800,11 @@
       </c>
       <c r="J29" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K29" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1837,11 +1837,11 @@
       </c>
       <c r="J30" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K30" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1874,11 +1874,11 @@
       </c>
       <c r="J31" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K31" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1907,15 +1907,14 @@
         <v>75</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J32" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>45059</v>
-      </c>
-      <c r="K32" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>54</v>
+      </c>
+      <c r="J32" s="7">
+        <v>45072</v>
+      </c>
+      <c r="K32" s="8">
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1948,11 +1947,11 @@
       </c>
       <c r="J33" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K33" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1985,11 +1984,11 @@
       </c>
       <c r="J34" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K34" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2022,11 +2021,11 @@
       </c>
       <c r="J35" s="4">
         <f t="shared" ref="J35:J41" ca="1" si="2">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K35" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2059,11 +2058,11 @@
       </c>
       <c r="J36" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K36" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2168,11 +2167,11 @@
       </c>
       <c r="J39" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K39" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -2205,11 +2204,11 @@
       </c>
       <c r="J40" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K40" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2242,11 +2241,11 @@
       </c>
       <c r="J41" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K41" s="6">
         <f t="shared" ref="K41:K44" ca="1" si="3">DATEDIF(A41,J41,"d")</f>
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -2315,11 +2314,11 @@
       </c>
       <c r="J43" s="4">
         <f ca="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K43" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -2352,11 +2351,11 @@
       </c>
       <c r="J44" s="4">
         <f ca="1">TODAY()</f>
-        <v>45059</v>
+        <v>45072</v>
       </c>
       <c r="K44" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>